<commit_message>
update overlay and tracker
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-high-microsoft-windows-server-2016-stig-overlay.xlsx
+++ b/cms-ars-3.1-high-microsoft-windows-server-2016-stig-overlay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\cms-ars3.1-windows2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishna/Documents/Projects/CMS/Inspec/STIG_Profiles/microsoft-windows-server-2016/cms-ars-3.1-high-microsoft-windows-server-2016-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8E33C6-4EF7-43AD-A72D-01E9919FD366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BED612-AE70-EF48-8A83-498F8B4019AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-high-microsoft-wind" sheetId="1" r:id="rId1"/>
@@ -32592,25 +32592,25 @@
   <dimension ref="A1:AF273"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E188" sqref="E188"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="30.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="31"/>
   <cols>
     <col min="1" max="1" width="9.5" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9.34765625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.19921875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="35.09765625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="35.1640625" style="6" customWidth="1"/>
     <col min="6" max="23" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="51.44921875" style="6" customWidth="1"/>
+    <col min="24" max="24" width="51.5" style="6" customWidth="1"/>
     <col min="25" max="25" width="48" style="6" customWidth="1"/>
     <col min="26" max="27" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="34.5" style="1" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="33.5" style="2" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="16.8984375" style="6" customWidth="1"/>
-    <col min="31" max="31" width="17.046875" style="7" customWidth="1"/>
+    <col min="30" max="30" width="16.83203125" style="6" customWidth="1"/>
+    <col min="31" max="31" width="17" style="7" customWidth="1"/>
     <col min="32" max="32" width="0" style="27" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -32710,7 +32710,7 @@
       </c>
       <c r="AF1" s="26"/>
     </row>
-    <row r="2" spans="1:32" ht="149.4" customHeight="1">
+    <row r="2" spans="1:32" ht="149.5" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>69</v>
       </c>
@@ -32777,7 +32777,7 @@
       </c>
       <c r="AE2" s="15"/>
     </row>
-    <row r="3" spans="1:32" ht="297.60000000000002" customHeight="1">
+    <row r="3" spans="1:32" ht="297.5" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>918</v>
       </c>
@@ -32844,7 +32844,7 @@
       </c>
       <c r="AE3" s="15"/>
     </row>
-    <row r="4" spans="1:32" ht="409.5">
+    <row r="4" spans="1:32" ht="409.6">
       <c r="A4" s="8" t="s">
         <v>2731</v>
       </c>
@@ -32911,7 +32911,7 @@
       </c>
       <c r="AE4" s="15"/>
     </row>
-    <row r="5" spans="1:32" ht="409.5">
+    <row r="5" spans="1:32" ht="409.6">
       <c r="A5" s="8" t="s">
         <v>83</v>
       </c>
@@ -32978,7 +32978,7 @@
       </c>
       <c r="AE5" s="15"/>
     </row>
-    <row r="6" spans="1:32" ht="409.5">
+    <row r="6" spans="1:32" ht="409.6">
       <c r="A6" s="8" t="s">
         <v>2624</v>
       </c>
@@ -33045,7 +33045,7 @@
       </c>
       <c r="AE6" s="15"/>
     </row>
-    <row r="7" spans="1:32" ht="409.5">
+    <row r="7" spans="1:32" ht="409.6">
       <c r="A7" s="8" t="s">
         <v>218</v>
       </c>
@@ -33112,7 +33112,7 @@
       </c>
       <c r="AE7" s="15"/>
     </row>
-    <row r="8" spans="1:32" ht="409.5">
+    <row r="8" spans="1:32" ht="409.6">
       <c r="A8" s="8" t="s">
         <v>631</v>
       </c>
@@ -33179,7 +33179,7 @@
       </c>
       <c r="AE8" s="15"/>
     </row>
-    <row r="9" spans="1:32" ht="409.5">
+    <row r="9" spans="1:32" ht="409.6">
       <c r="A9" s="9" t="s">
         <v>2763</v>
       </c>
@@ -33249,7 +33249,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="409.5">
+    <row r="10" spans="1:32" ht="409.6">
       <c r="A10" s="8" t="s">
         <v>147</v>
       </c>
@@ -33316,7 +33316,7 @@
       </c>
       <c r="AE10" s="15"/>
     </row>
-    <row r="11" spans="1:32" ht="409.5">
+    <row r="11" spans="1:32" ht="409.6">
       <c r="A11" s="9" t="s">
         <v>2658</v>
       </c>
@@ -33387,7 +33387,7 @@
         <v>3128</v>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="409.5">
+    <row r="12" spans="1:32" ht="409.6">
       <c r="A12" s="8" t="s">
         <v>274</v>
       </c>
@@ -33454,7 +33454,7 @@
       </c>
       <c r="AE12" s="15"/>
     </row>
-    <row r="13" spans="1:32" ht="409.5">
+    <row r="13" spans="1:32" ht="409.6">
       <c r="A13" s="8" t="s">
         <v>896</v>
       </c>
@@ -33521,7 +33521,7 @@
       </c>
       <c r="AE13" s="15"/>
     </row>
-    <row r="14" spans="1:32" ht="409.5">
+    <row r="14" spans="1:32" ht="409.6">
       <c r="A14" s="8" t="s">
         <v>3002</v>
       </c>
@@ -33588,7 +33588,7 @@
       </c>
       <c r="AE14" s="15"/>
     </row>
-    <row r="15" spans="1:32" ht="409.5">
+    <row r="15" spans="1:32" ht="409.6">
       <c r="A15" s="8" t="s">
         <v>2836</v>
       </c>
@@ -33655,7 +33655,7 @@
       </c>
       <c r="AE15" s="15"/>
     </row>
-    <row r="16" spans="1:32" ht="409.5">
+    <row r="16" spans="1:32" ht="409.6">
       <c r="A16" s="8" t="s">
         <v>511</v>
       </c>
@@ -33722,7 +33722,7 @@
       </c>
       <c r="AE16" s="15"/>
     </row>
-    <row r="17" spans="1:32" ht="409.5">
+    <row r="17" spans="1:32" ht="409.6">
       <c r="A17" s="8" t="s">
         <v>1185</v>
       </c>
@@ -33791,7 +33791,7 @@
       </c>
       <c r="AE17" s="15"/>
     </row>
-    <row r="18" spans="1:32" ht="409.5">
+    <row r="18" spans="1:32" ht="409.6">
       <c r="A18" s="8" t="s">
         <v>3011</v>
       </c>
@@ -33860,7 +33860,7 @@
       </c>
       <c r="AE18" s="15"/>
     </row>
-    <row r="19" spans="1:32" ht="409.5">
+    <row r="19" spans="1:32" ht="409.6">
       <c r="A19" s="8" t="s">
         <v>392</v>
       </c>
@@ -33929,7 +33929,7 @@
       </c>
       <c r="AE19" s="15"/>
     </row>
-    <row r="20" spans="1:32" ht="409.5">
+    <row r="20" spans="1:32" ht="409.6">
       <c r="A20" s="8" t="s">
         <v>2902</v>
       </c>
@@ -33996,7 +33996,7 @@
       </c>
       <c r="AE20" s="15"/>
     </row>
-    <row r="21" spans="1:32" ht="409.5">
+    <row r="21" spans="1:32" ht="409.6">
       <c r="A21" s="8" t="s">
         <v>587</v>
       </c>
@@ -34063,7 +34063,7 @@
       </c>
       <c r="AE21" s="15"/>
     </row>
-    <row r="22" spans="1:32" ht="409.5">
+    <row r="22" spans="1:32" ht="409.6">
       <c r="A22" s="9" t="s">
         <v>1395</v>
       </c>
@@ -34132,7 +34132,7 @@
       </c>
       <c r="AE22" s="15"/>
     </row>
-    <row r="23" spans="1:32" ht="409.5">
+    <row r="23" spans="1:32" ht="409.6">
       <c r="A23" s="8" t="s">
         <v>2877</v>
       </c>
@@ -34199,7 +34199,7 @@
       </c>
       <c r="AE23" s="15"/>
     </row>
-    <row r="24" spans="1:32" ht="409.5">
+    <row r="24" spans="1:32" ht="409.6">
       <c r="A24" s="8" t="s">
         <v>576</v>
       </c>
@@ -34266,7 +34266,7 @@
       </c>
       <c r="AE24" s="15"/>
     </row>
-    <row r="25" spans="1:32" ht="409.5">
+    <row r="25" spans="1:32" ht="409.6">
       <c r="A25" s="9" t="s">
         <v>3047</v>
       </c>
@@ -34337,7 +34337,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="26" spans="1:32" ht="409.5">
+    <row r="26" spans="1:32" ht="409.6">
       <c r="A26" s="8" t="s">
         <v>429</v>
       </c>
@@ -34404,7 +34404,7 @@
       </c>
       <c r="AE26" s="15"/>
     </row>
-    <row r="27" spans="1:32" ht="409.5">
+    <row r="27" spans="1:32" ht="409.6">
       <c r="A27" s="8" t="s">
         <v>2858</v>
       </c>
@@ -34471,7 +34471,7 @@
       </c>
       <c r="AE27" s="15"/>
     </row>
-    <row r="28" spans="1:32" ht="409.5">
+    <row r="28" spans="1:32" ht="409.6">
       <c r="A28" s="8" t="s">
         <v>525</v>
       </c>
@@ -34540,7 +34540,7 @@
       </c>
       <c r="AE28" s="15"/>
     </row>
-    <row r="29" spans="1:32" ht="409.5">
+    <row r="29" spans="1:32" ht="409.6">
       <c r="A29" s="9" t="s">
         <v>2977</v>
       </c>
@@ -34613,7 +34613,7 @@
         <v>3128</v>
       </c>
     </row>
-    <row r="30" spans="1:32" ht="409.5">
+    <row r="30" spans="1:32" ht="409.6">
       <c r="A30" s="8" t="s">
         <v>344</v>
       </c>
@@ -34680,7 +34680,7 @@
       </c>
       <c r="AE30" s="15"/>
     </row>
-    <row r="31" spans="1:32" ht="409.5">
+    <row r="31" spans="1:32" ht="409.6">
       <c r="A31" s="8" t="s">
         <v>1421</v>
       </c>
@@ -34747,7 +34747,7 @@
       </c>
       <c r="AE31" s="15"/>
     </row>
-    <row r="32" spans="1:32" ht="409.5">
+    <row r="32" spans="1:32" ht="409.6">
       <c r="A32" s="9" t="s">
         <v>110</v>
       </c>
@@ -34817,7 +34817,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="33" spans="1:32" ht="409.5">
+    <row r="33" spans="1:32" ht="409.6">
       <c r="A33" s="9" t="s">
         <v>2721</v>
       </c>
@@ -34884,7 +34884,7 @@
       </c>
       <c r="AE33" s="15"/>
     </row>
-    <row r="34" spans="1:32" ht="409.5">
+    <row r="34" spans="1:32" ht="409.6">
       <c r="A34" s="9" t="s">
         <v>240</v>
       </c>
@@ -34954,7 +34954,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="35" spans="1:32" ht="409.5">
+    <row r="35" spans="1:32" ht="409.6">
       <c r="A35" s="8" t="s">
         <v>2613</v>
       </c>
@@ -35021,7 +35021,7 @@
       </c>
       <c r="AE35" s="15"/>
     </row>
-    <row r="36" spans="1:32" ht="409.5">
+    <row r="36" spans="1:32" ht="409.6">
       <c r="A36" s="8" t="s">
         <v>1894</v>
       </c>
@@ -35088,7 +35088,7 @@
       </c>
       <c r="AE36" s="15"/>
     </row>
-    <row r="37" spans="1:32" ht="409.5">
+    <row r="37" spans="1:32" ht="409.6">
       <c r="A37" s="8" t="s">
         <v>121</v>
       </c>
@@ -35155,7 +35155,7 @@
       </c>
       <c r="AE37" s="15"/>
     </row>
-    <row r="38" spans="1:32" ht="409.5">
+    <row r="38" spans="1:32" ht="409.6">
       <c r="A38" s="8" t="s">
         <v>2770</v>
       </c>
@@ -35222,7 +35222,7 @@
       </c>
       <c r="AE38" s="15"/>
     </row>
-    <row r="39" spans="1:32" ht="409.5">
+    <row r="39" spans="1:32" ht="409.6">
       <c r="A39" s="8" t="s">
         <v>250</v>
       </c>
@@ -35289,7 +35289,7 @@
       </c>
       <c r="AE39" s="15"/>
     </row>
-    <row r="40" spans="1:32" ht="409.5">
+    <row r="40" spans="1:32" ht="409.6">
       <c r="A40" s="8" t="s">
         <v>2669</v>
       </c>
@@ -35356,7 +35356,7 @@
       </c>
       <c r="AE40" s="15"/>
     </row>
-    <row r="41" spans="1:32" ht="409.5">
+    <row r="41" spans="1:32" ht="409.6">
       <c r="A41" s="8" t="s">
         <v>2118</v>
       </c>
@@ -35423,7 +35423,7 @@
       </c>
       <c r="AE41" s="15"/>
     </row>
-    <row r="42" spans="1:32" ht="409.5">
+    <row r="42" spans="1:32" ht="409.6">
       <c r="A42" s="8" t="s">
         <v>2991</v>
       </c>
@@ -35490,7 +35490,7 @@
       </c>
       <c r="AE42" s="15"/>
     </row>
-    <row r="43" spans="1:32" ht="409.5">
+    <row r="43" spans="1:32" ht="409.6">
       <c r="A43" s="8" t="s">
         <v>366</v>
       </c>
@@ -35557,7 +35557,7 @@
       </c>
       <c r="AE43" s="15"/>
     </row>
-    <row r="44" spans="1:32" ht="409.5">
+    <row r="44" spans="1:32" ht="409.6">
       <c r="A44" s="8" t="s">
         <v>2825</v>
       </c>
@@ -35624,7 +35624,7 @@
       </c>
       <c r="AE44" s="15"/>
     </row>
-    <row r="45" spans="1:32" ht="409.5">
+    <row r="45" spans="1:32" ht="409.6">
       <c r="A45" s="9" t="s">
         <v>499</v>
       </c>
@@ -35694,7 +35694,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="46" spans="1:32" ht="409.5">
+    <row r="46" spans="1:32" ht="409.6">
       <c r="A46" s="9" t="s">
         <v>1176</v>
       </c>
@@ -35761,7 +35761,7 @@
       </c>
       <c r="AE46" s="15"/>
     </row>
-    <row r="47" spans="1:32" ht="409.5">
+    <row r="47" spans="1:32" ht="409.6">
       <c r="A47" s="8" t="s">
         <v>3022</v>
       </c>
@@ -35828,7 +35828,7 @@
       </c>
       <c r="AE47" s="15"/>
     </row>
-    <row r="48" spans="1:32" ht="409.5">
+    <row r="48" spans="1:32" ht="409.6">
       <c r="A48" s="9" t="s">
         <v>406</v>
       </c>
@@ -35897,7 +35897,7 @@
       </c>
       <c r="AE48" s="15"/>
     </row>
-    <row r="49" spans="1:31" ht="409.5">
+    <row r="49" spans="1:31" ht="409.6">
       <c r="A49" s="9" t="s">
         <v>2912</v>
       </c>
@@ -35964,7 +35964,7 @@
       </c>
       <c r="AE49" s="15"/>
     </row>
-    <row r="50" spans="1:31" ht="409.5">
+    <row r="50" spans="1:31" ht="409.6">
       <c r="A50" s="8" t="s">
         <v>598</v>
       </c>
@@ -36031,7 +36031,7 @@
       </c>
       <c r="AE50" s="15"/>
     </row>
-    <row r="51" spans="1:31" ht="409.5">
+    <row r="51" spans="1:31" ht="409.6">
       <c r="A51" s="8" t="s">
         <v>1408</v>
       </c>
@@ -36098,7 +36098,7 @@
       </c>
       <c r="AE51" s="15"/>
     </row>
-    <row r="52" spans="1:31" ht="409.5">
+    <row r="52" spans="1:31" ht="409.6">
       <c r="A52" s="9" t="s">
         <v>2868</v>
       </c>
@@ -36165,7 +36165,7 @@
       </c>
       <c r="AE52" s="15"/>
     </row>
-    <row r="53" spans="1:31" ht="409.5">
+    <row r="53" spans="1:31" ht="409.6">
       <c r="A53" s="8" t="s">
         <v>562</v>
       </c>
@@ -36234,7 +36234,7 @@
       </c>
       <c r="AE53" s="15"/>
     </row>
-    <row r="54" spans="1:31" ht="409.5">
+    <row r="54" spans="1:31" ht="409.6">
       <c r="A54" s="8" t="s">
         <v>3035</v>
       </c>
@@ -36301,7 +36301,7 @@
       </c>
       <c r="AE54" s="15"/>
     </row>
-    <row r="55" spans="1:31" ht="409.5">
+    <row r="55" spans="1:31" ht="409.6">
       <c r="A55" s="8" t="s">
         <v>907</v>
       </c>
@@ -36370,7 +36370,7 @@
       </c>
       <c r="AE55" s="15"/>
     </row>
-    <row r="56" spans="1:31" ht="409.5">
+    <row r="56" spans="1:31" ht="409.6">
       <c r="A56" s="8" t="s">
         <v>2742</v>
       </c>
@@ -36439,7 +36439,7 @@
       </c>
       <c r="AE56" s="15"/>
     </row>
-    <row r="57" spans="1:31" ht="409.5">
+    <row r="57" spans="1:31" ht="409.6">
       <c r="A57" s="8" t="s">
         <v>97</v>
       </c>
@@ -36508,7 +36508,7 @@
       </c>
       <c r="AE57" s="15"/>
     </row>
-    <row r="58" spans="1:31" ht="409.5">
+    <row r="58" spans="1:31" ht="409.6">
       <c r="A58" s="8" t="s">
         <v>2635</v>
       </c>
@@ -36577,7 +36577,7 @@
       </c>
       <c r="AE58" s="15"/>
     </row>
-    <row r="59" spans="1:31" ht="409.5">
+    <row r="59" spans="1:31" ht="409.6">
       <c r="A59" s="8" t="s">
         <v>229</v>
       </c>
@@ -36646,7 +36646,7 @@
       </c>
       <c r="AE59" s="15"/>
     </row>
-    <row r="60" spans="1:31" ht="409.5">
+    <row r="60" spans="1:31" ht="409.6">
       <c r="A60" s="8" t="s">
         <v>642</v>
       </c>
@@ -36713,7 +36713,7 @@
       </c>
       <c r="AE60" s="15"/>
     </row>
-    <row r="61" spans="1:31" ht="409.5">
+    <row r="61" spans="1:31" ht="409.6">
       <c r="A61" s="8" t="s">
         <v>2753</v>
       </c>
@@ -36780,7 +36780,7 @@
       </c>
       <c r="AE61" s="15"/>
     </row>
-    <row r="62" spans="1:31" ht="409.5">
+    <row r="62" spans="1:31" ht="409.6">
       <c r="A62" s="8" t="s">
         <v>133</v>
       </c>
@@ -36847,7 +36847,7 @@
       </c>
       <c r="AE62" s="15"/>
     </row>
-    <row r="63" spans="1:31" ht="409.5">
+    <row r="63" spans="1:31" ht="409.6">
       <c r="A63" s="8" t="s">
         <v>2646</v>
       </c>
@@ -36914,7 +36914,7 @@
       </c>
       <c r="AE63" s="15"/>
     </row>
-    <row r="64" spans="1:31" ht="409.5">
+    <row r="64" spans="1:31" ht="409.6">
       <c r="A64" s="8" t="s">
         <v>263</v>
       </c>
@@ -36981,7 +36981,7 @@
       </c>
       <c r="AE64" s="15"/>
     </row>
-    <row r="65" spans="1:31" ht="409.5">
+    <row r="65" spans="1:31" ht="409.6">
       <c r="A65" s="8" t="s">
         <v>885</v>
       </c>
@@ -37048,7 +37048,7 @@
       </c>
       <c r="AE65" s="15"/>
     </row>
-    <row r="66" spans="1:31" ht="409.5">
+    <row r="66" spans="1:31" ht="409.6">
       <c r="A66" s="8" t="s">
         <v>550</v>
       </c>
@@ -37115,7 +37115,7 @@
       </c>
       <c r="AE66" s="15"/>
     </row>
-    <row r="67" spans="1:31" ht="409.5">
+    <row r="67" spans="1:31" ht="409.6">
       <c r="A67" s="8" t="s">
         <v>2889</v>
       </c>
@@ -37182,7 +37182,7 @@
       </c>
       <c r="AE67" s="15"/>
     </row>
-    <row r="68" spans="1:31" ht="409.5">
+    <row r="68" spans="1:31" ht="409.6">
       <c r="A68" s="8" t="s">
         <v>418</v>
       </c>
@@ -37249,7 +37249,7 @@
       </c>
       <c r="AE68" s="15"/>
     </row>
-    <row r="69" spans="1:31" ht="409.5">
+    <row r="69" spans="1:31" ht="409.6">
       <c r="A69" s="9" t="s">
         <v>3060</v>
       </c>
@@ -37316,7 +37316,7 @@
       </c>
       <c r="AE69" s="15"/>
     </row>
-    <row r="70" spans="1:31" ht="409.5">
+    <row r="70" spans="1:31" ht="409.6">
       <c r="A70" s="8" t="s">
         <v>2339</v>
       </c>
@@ -37385,7 +37385,7 @@
       </c>
       <c r="AE70" s="15"/>
     </row>
-    <row r="71" spans="1:31" ht="409.5">
+    <row r="71" spans="1:31" ht="409.6">
       <c r="A71" s="8" t="s">
         <v>539</v>
       </c>
@@ -37454,7 +37454,7 @@
       </c>
       <c r="AE71" s="15"/>
     </row>
-    <row r="72" spans="1:31" ht="409.5">
+    <row r="72" spans="1:31" ht="409.6">
       <c r="A72" s="8" t="s">
         <v>2847</v>
       </c>
@@ -37523,7 +37523,7 @@
       </c>
       <c r="AE72" s="15"/>
     </row>
-    <row r="73" spans="1:31" ht="409.5">
+    <row r="73" spans="1:31" ht="409.6">
       <c r="A73" s="8" t="s">
         <v>355</v>
       </c>
@@ -37592,7 +37592,7 @@
       </c>
       <c r="AE73" s="15"/>
     </row>
-    <row r="74" spans="1:31" ht="409.5">
+    <row r="74" spans="1:31" ht="409.6">
       <c r="A74" s="8" t="s">
         <v>2965</v>
       </c>
@@ -37661,7 +37661,7 @@
       </c>
       <c r="AE74" s="15"/>
     </row>
-    <row r="75" spans="1:31" ht="409.5">
+    <row r="75" spans="1:31" ht="409.6">
       <c r="A75" s="8" t="s">
         <v>2129</v>
       </c>
@@ -37730,7 +37730,7 @@
       </c>
       <c r="AE75" s="15"/>
     </row>
-    <row r="76" spans="1:31" ht="409.5">
+    <row r="76" spans="1:31" ht="409.6">
       <c r="A76" s="9" t="s">
         <v>2028</v>
       </c>
@@ -37801,7 +37801,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="77" spans="1:31" ht="409.5">
+    <row r="77" spans="1:31" ht="409.6">
       <c r="A77" s="9" t="s">
         <v>791</v>
       </c>
@@ -37872,7 +37872,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="78" spans="1:31" ht="409.5">
+    <row r="78" spans="1:31" ht="409.6">
       <c r="A78" s="8" t="s">
         <v>1844</v>
       </c>
@@ -37941,7 +37941,7 @@
       </c>
       <c r="AE78" s="15"/>
     </row>
-    <row r="79" spans="1:31" ht="409.5">
+    <row r="79" spans="1:31" ht="409.6">
       <c r="A79" s="8" t="s">
         <v>1165</v>
       </c>
@@ -38010,7 +38010,7 @@
       </c>
       <c r="AE79" s="15"/>
     </row>
-    <row r="80" spans="1:31" ht="409.5">
+    <row r="80" spans="1:31" ht="409.6">
       <c r="A80" s="8" t="s">
         <v>175</v>
       </c>
@@ -38079,7 +38079,7 @@
       </c>
       <c r="AE80" s="15"/>
     </row>
-    <row r="81" spans="1:31" ht="409.5">
+    <row r="81" spans="1:31" ht="409.6">
       <c r="A81" s="8" t="s">
         <v>1968</v>
       </c>
@@ -38148,7 +38148,7 @@
       </c>
       <c r="AE81" s="15"/>
     </row>
-    <row r="82" spans="1:31" ht="409.5">
+    <row r="82" spans="1:31" ht="409.6">
       <c r="A82" s="8" t="s">
         <v>710</v>
       </c>
@@ -38215,7 +38215,7 @@
       </c>
       <c r="AE82" s="15"/>
     </row>
-    <row r="83" spans="1:31" ht="409.5">
+    <row r="83" spans="1:31" ht="409.6">
       <c r="A83" s="8" t="s">
         <v>1703</v>
       </c>
@@ -38282,7 +38282,7 @@
       </c>
       <c r="AE83" s="15"/>
     </row>
-    <row r="84" spans="1:31" ht="409.5">
+    <row r="84" spans="1:31" ht="409.6">
       <c r="A84" s="8" t="s">
         <v>929</v>
       </c>
@@ -38351,7 +38351,7 @@
       </c>
       <c r="AE84" s="15"/>
     </row>
-    <row r="85" spans="1:31" ht="409.5">
+    <row r="85" spans="1:31" ht="409.6">
       <c r="A85" s="8" t="s">
         <v>40</v>
       </c>
@@ -38420,7 +38420,7 @@
       </c>
       <c r="AE85" s="15"/>
     </row>
-    <row r="86" spans="1:31" ht="409.5">
+    <row r="86" spans="1:31" ht="409.6">
       <c r="A86" s="8" t="s">
         <v>1000</v>
       </c>
@@ -38489,7 +38489,7 @@
       </c>
       <c r="AE86" s="15"/>
     </row>
-    <row r="87" spans="1:31" ht="409.5">
+    <row r="87" spans="1:31" ht="409.6">
       <c r="A87" s="8" t="s">
         <v>666</v>
       </c>
@@ -38558,7 +38558,7 @@
       </c>
       <c r="AE87" s="15"/>
     </row>
-    <row r="88" spans="1:31" ht="409.5">
+    <row r="88" spans="1:31" ht="409.6">
       <c r="A88" s="8" t="s">
         <v>204</v>
       </c>
@@ -38627,7 +38627,7 @@
       </c>
       <c r="AE88" s="15"/>
     </row>
-    <row r="89" spans="1:31" ht="409.5">
+    <row r="89" spans="1:31" ht="409.6">
       <c r="A89" s="8" t="s">
         <v>1770</v>
       </c>
@@ -38694,7 +38694,7 @@
       </c>
       <c r="AE89" s="15"/>
     </row>
-    <row r="90" spans="1:31" ht="409.5">
+    <row r="90" spans="1:31" ht="409.6">
       <c r="A90" s="8" t="s">
         <v>1092</v>
       </c>
@@ -38763,7 +38763,7 @@
       </c>
       <c r="AE90" s="15"/>
     </row>
-    <row r="91" spans="1:31" ht="409.5">
+    <row r="91" spans="1:31" ht="409.6">
       <c r="A91" s="8" t="s">
         <v>2059</v>
       </c>
@@ -38832,7 +38832,7 @@
       </c>
       <c r="AE91" s="15"/>
     </row>
-    <row r="92" spans="1:31" ht="409.5">
+    <row r="92" spans="1:31" ht="409.6">
       <c r="A92" s="8" t="s">
         <v>863</v>
       </c>
@@ -38901,7 +38901,7 @@
       </c>
       <c r="AE92" s="15"/>
     </row>
-    <row r="93" spans="1:31" ht="409.5">
+    <row r="93" spans="1:31" ht="409.6">
       <c r="A93" s="8" t="s">
         <v>285</v>
       </c>
@@ -38970,7 +38970,7 @@
       </c>
       <c r="AE93" s="15"/>
     </row>
-    <row r="94" spans="1:31" ht="409.5">
+    <row r="94" spans="1:31" ht="409.6">
       <c r="A94" s="8" t="s">
         <v>2207</v>
       </c>
@@ -39039,7 +39039,7 @@
       </c>
       <c r="AE94" s="15"/>
     </row>
-    <row r="95" spans="1:31" ht="409.5">
+    <row r="95" spans="1:31" ht="409.6">
       <c r="A95" s="8" t="s">
         <v>1486</v>
       </c>
@@ -39108,7 +39108,7 @@
       </c>
       <c r="AE95" s="15"/>
     </row>
-    <row r="96" spans="1:31" ht="409.5">
+    <row r="96" spans="1:31" ht="409.6">
       <c r="A96" s="8" t="s">
         <v>2390</v>
       </c>
@@ -39177,7 +39177,7 @@
       </c>
       <c r="AE96" s="15"/>
     </row>
-    <row r="97" spans="1:31" ht="409.5">
+    <row r="97" spans="1:31" ht="409.6">
       <c r="A97" s="8" t="s">
         <v>1207</v>
       </c>
@@ -39244,7 +39244,7 @@
       </c>
       <c r="AE97" s="15"/>
     </row>
-    <row r="98" spans="1:31" ht="409.5">
+    <row r="98" spans="1:31" ht="409.6">
       <c r="A98" s="8" t="s">
         <v>463</v>
       </c>
@@ -39313,7 +39313,7 @@
       </c>
       <c r="AE98" s="15"/>
     </row>
-    <row r="99" spans="1:31" ht="409.5">
+    <row r="99" spans="1:31" ht="409.6">
       <c r="A99" s="8" t="s">
         <v>2238</v>
       </c>
@@ -39382,7 +39382,7 @@
       </c>
       <c r="AE99" s="15"/>
     </row>
-    <row r="100" spans="1:31" ht="409.5">
+    <row r="100" spans="1:31" ht="409.6">
       <c r="A100" s="8" t="s">
         <v>1580</v>
       </c>
@@ -39451,7 +39451,7 @@
       </c>
       <c r="AE100" s="15"/>
     </row>
-    <row r="101" spans="1:31" ht="409.5">
+    <row r="101" spans="1:31" ht="409.6">
       <c r="A101" s="8" t="s">
         <v>2550</v>
       </c>
@@ -39520,7 +39520,7 @@
       </c>
       <c r="AE101" s="15"/>
     </row>
-    <row r="102" spans="1:31" ht="409.5">
+    <row r="102" spans="1:31" ht="409.6">
       <c r="A102" s="8" t="s">
         <v>1373</v>
       </c>
@@ -39587,7 +39587,7 @@
       </c>
       <c r="AE102" s="15"/>
     </row>
-    <row r="103" spans="1:31" ht="409.5">
+    <row r="103" spans="1:31" ht="409.6">
       <c r="A103" s="8" t="s">
         <v>621</v>
       </c>
@@ -39654,7 +39654,7 @@
       </c>
       <c r="AE103" s="15"/>
     </row>
-    <row r="104" spans="1:31" ht="409.5">
+    <row r="104" spans="1:31" ht="409.6">
       <c r="A104" s="8" t="s">
         <v>2475</v>
       </c>
@@ -39723,7 +39723,7 @@
       </c>
       <c r="AE104" s="15"/>
     </row>
-    <row r="105" spans="1:31" ht="409.5">
+    <row r="105" spans="1:31" ht="409.6">
       <c r="A105" s="8" t="s">
         <v>1342</v>
       </c>
@@ -39792,7 +39792,7 @@
       </c>
       <c r="AE105" s="15"/>
     </row>
-    <row r="106" spans="1:31" ht="409.5">
+    <row r="106" spans="1:31" ht="409.6">
       <c r="A106" s="8" t="s">
         <v>2282</v>
       </c>
@@ -39861,7 +39861,7 @@
       </c>
       <c r="AE106" s="15"/>
     </row>
-    <row r="107" spans="1:31" ht="409.5">
+    <row r="107" spans="1:31" ht="409.6">
       <c r="A107" s="8" t="s">
         <v>1641</v>
       </c>
@@ -39930,7 +39930,7 @@
       </c>
       <c r="AE107" s="15"/>
     </row>
-    <row r="108" spans="1:31" ht="409.5">
+    <row r="108" spans="1:31" ht="409.6">
       <c r="A108" s="8" t="s">
         <v>440</v>
       </c>
@@ -39999,7 +39999,7 @@
       </c>
       <c r="AE108" s="15"/>
     </row>
-    <row r="109" spans="1:31" ht="409.5">
+    <row r="109" spans="1:31" ht="409.6">
       <c r="A109" s="8" t="s">
         <v>2466</v>
       </c>
@@ -40068,7 +40068,7 @@
       </c>
       <c r="AE109" s="15"/>
     </row>
-    <row r="110" spans="1:31" ht="409.5">
+    <row r="110" spans="1:31" ht="409.6">
       <c r="A110" s="8" t="s">
         <v>1251</v>
       </c>
@@ -40137,7 +40137,7 @@
       </c>
       <c r="AE110" s="15"/>
     </row>
-    <row r="111" spans="1:31" ht="409.5">
+    <row r="111" spans="1:31" ht="409.6">
       <c r="A111" s="8" t="s">
         <v>2176</v>
       </c>
@@ -40206,7 +40206,7 @@
       </c>
       <c r="AE111" s="15"/>
     </row>
-    <row r="112" spans="1:31" ht="409.5">
+    <row r="112" spans="1:31" ht="409.6">
       <c r="A112" s="8" t="s">
         <v>1443</v>
       </c>
@@ -40275,7 +40275,7 @@
       </c>
       <c r="AE112" s="15"/>
     </row>
-    <row r="113" spans="1:31" ht="409.5">
+    <row r="113" spans="1:31" ht="409.6">
       <c r="A113" s="8" t="s">
         <v>333</v>
       </c>
@@ -40344,7 +40344,7 @@
       </c>
       <c r="AE113" s="15"/>
     </row>
-    <row r="114" spans="1:31" ht="409.5">
+    <row r="114" spans="1:31" ht="409.6">
       <c r="A114" s="8" t="s">
         <v>1036</v>
       </c>
@@ -40413,7 +40413,7 @@
       </c>
       <c r="AE114" s="15"/>
     </row>
-    <row r="115" spans="1:31" ht="409.5">
+    <row r="115" spans="1:31" ht="409.6">
       <c r="A115" s="8" t="s">
         <v>1723</v>
       </c>
@@ -40482,7 +40482,7 @@
       </c>
       <c r="AE115" s="15"/>
     </row>
-    <row r="116" spans="1:31" ht="409.5">
+    <row r="116" spans="1:31" ht="409.6">
       <c r="A116" s="8" t="s">
         <v>1923</v>
       </c>
@@ -40549,7 +40549,7 @@
       </c>
       <c r="AE116" s="15"/>
     </row>
-    <row r="117" spans="1:31" ht="409.5">
+    <row r="117" spans="1:31" ht="409.6">
       <c r="A117" s="8" t="s">
         <v>2582</v>
       </c>
@@ -40618,7 +40618,7 @@
       </c>
       <c r="AE117" s="15"/>
     </row>
-    <row r="118" spans="1:31" ht="409.5">
+    <row r="118" spans="1:31" ht="409.6">
       <c r="A118" s="8" t="s">
         <v>1047</v>
       </c>
@@ -40687,7 +40687,7 @@
       </c>
       <c r="AE118" s="15"/>
     </row>
-    <row r="119" spans="1:31" ht="409.5">
+    <row r="119" spans="1:31" ht="409.6">
       <c r="A119" s="8" t="s">
         <v>1822</v>
       </c>
@@ -40754,7 +40754,7 @@
       </c>
       <c r="AE119" s="15"/>
     </row>
-    <row r="120" spans="1:31" ht="409.5">
+    <row r="120" spans="1:31" ht="409.6">
       <c r="A120" s="8" t="s">
         <v>850</v>
       </c>
@@ -40821,7 +40821,7 @@
       </c>
       <c r="AE120" s="15"/>
     </row>
-    <row r="121" spans="1:31" ht="409.5">
+    <row r="121" spans="1:31" ht="409.6">
       <c r="A121" s="8" t="s">
         <v>2081</v>
       </c>
@@ -40888,7 +40888,7 @@
       </c>
       <c r="AE121" s="15"/>
     </row>
-    <row r="122" spans="1:31" ht="409.5">
+    <row r="122" spans="1:31" ht="409.6">
       <c r="A122" s="8" t="s">
         <v>2691</v>
       </c>
@@ -40955,7 +40955,7 @@
       </c>
       <c r="AE122" s="15"/>
     </row>
-    <row r="123" spans="1:31" ht="409.5">
+    <row r="123" spans="1:31" ht="409.6">
       <c r="A123" s="8" t="s">
         <v>2218</v>
       </c>
@@ -41022,7 +41022,7 @@
       </c>
       <c r="AE123" s="15"/>
     </row>
-    <row r="124" spans="1:31" ht="409.5">
+    <row r="124" spans="1:31" ht="409.6">
       <c r="A124" s="8" t="s">
         <v>1500</v>
       </c>
@@ -41089,7 +41089,7 @@
       </c>
       <c r="AE124" s="15"/>
     </row>
-    <row r="125" spans="1:31" ht="409.5">
+    <row r="125" spans="1:31" ht="409.6">
       <c r="A125" s="8" t="s">
         <v>2402</v>
       </c>
@@ -41156,7 +41156,7 @@
       </c>
       <c r="AE125" s="15"/>
     </row>
-    <row r="126" spans="1:31" ht="409.5">
+    <row r="126" spans="1:31" ht="409.6">
       <c r="A126" s="8" t="s">
         <v>1218</v>
       </c>
@@ -41223,7 +41223,7 @@
       </c>
       <c r="AE126" s="15"/>
     </row>
-    <row r="127" spans="1:31" ht="409.5">
+    <row r="127" spans="1:31" ht="409.6">
       <c r="A127" s="8" t="s">
         <v>477</v>
       </c>
@@ -41290,7 +41290,7 @@
       </c>
       <c r="AE127" s="15"/>
     </row>
-    <row r="128" spans="1:31" ht="409.5">
+    <row r="128" spans="1:31" ht="409.6">
       <c r="A128" s="8" t="s">
         <v>2229</v>
       </c>
@@ -41357,7 +41357,7 @@
       </c>
       <c r="AE128" s="15"/>
     </row>
-    <row r="129" spans="1:31" ht="409.5">
+    <row r="129" spans="1:31" ht="409.6">
       <c r="A129" s="8" t="s">
         <v>1569</v>
       </c>
@@ -41424,7 +41424,7 @@
       </c>
       <c r="AE129" s="15"/>
     </row>
-    <row r="130" spans="1:31" ht="409.5">
+    <row r="130" spans="1:31" ht="409.6">
       <c r="A130" s="8" t="s">
         <v>2539</v>
       </c>
@@ -41491,7 +41491,7 @@
       </c>
       <c r="AE130" s="15"/>
     </row>
-    <row r="131" spans="1:31" ht="409.5">
+    <row r="131" spans="1:31" ht="409.6">
       <c r="A131" s="8" t="s">
         <v>2486</v>
       </c>
@@ -41558,7 +41558,7 @@
       </c>
       <c r="AE131" s="15"/>
     </row>
-    <row r="132" spans="1:31" ht="409.5">
+    <row r="132" spans="1:31" ht="409.6">
       <c r="A132" s="8" t="s">
         <v>2293</v>
       </c>
@@ -41625,7 +41625,7 @@
       </c>
       <c r="AE132" s="15"/>
     </row>
-    <row r="133" spans="1:31" ht="409.5">
+    <row r="133" spans="1:31" ht="409.6">
       <c r="A133" s="8" t="s">
         <v>1652</v>
       </c>
@@ -41692,7 +41692,7 @@
       </c>
       <c r="AE133" s="15"/>
     </row>
-    <row r="134" spans="1:31" ht="409.5">
+    <row r="134" spans="1:31" ht="409.6">
       <c r="A134" s="8" t="s">
         <v>451</v>
       </c>
@@ -41759,7 +41759,7 @@
       </c>
       <c r="AE134" s="15"/>
     </row>
-    <row r="135" spans="1:31" ht="409.5">
+    <row r="135" spans="1:31" ht="409.6">
       <c r="A135" s="8" t="s">
         <v>2457</v>
       </c>
@@ -41826,7 +41826,7 @@
       </c>
       <c r="AE135" s="15"/>
     </row>
-    <row r="136" spans="1:31" ht="409.5">
+    <row r="136" spans="1:31" ht="409.6">
       <c r="A136" s="8" t="s">
         <v>1240</v>
       </c>
@@ -41893,7 +41893,7 @@
       </c>
       <c r="AE136" s="15"/>
     </row>
-    <row r="137" spans="1:31" ht="409.5">
+    <row r="137" spans="1:31" ht="409.6">
       <c r="A137" s="8" t="s">
         <v>1434</v>
       </c>
@@ -41960,7 +41960,7 @@
       </c>
       <c r="AE137" s="15"/>
     </row>
-    <row r="138" spans="1:31" ht="409.5">
+    <row r="138" spans="1:31" ht="409.6">
       <c r="A138" s="8" t="s">
         <v>322</v>
       </c>
@@ -42027,7 +42027,7 @@
       </c>
       <c r="AE138" s="15"/>
     </row>
-    <row r="139" spans="1:31" ht="409.5">
+    <row r="139" spans="1:31" ht="409.6">
       <c r="A139" s="9" t="s">
         <v>2016</v>
       </c>
@@ -42098,7 +42098,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="140" spans="1:31" ht="409.5">
+    <row r="140" spans="1:31" ht="409.6">
       <c r="A140" s="8" t="s">
         <v>779</v>
       </c>
@@ -42165,7 +42165,7 @@
       </c>
       <c r="AE140" s="15"/>
     </row>
-    <row r="141" spans="1:31" ht="409.5">
+    <row r="141" spans="1:31" ht="409.6">
       <c r="A141" s="8" t="s">
         <v>1833</v>
       </c>
@@ -42232,7 +42232,7 @@
       </c>
       <c r="AE141" s="15"/>
     </row>
-    <row r="142" spans="1:31" ht="409.5">
+    <row r="142" spans="1:31" ht="409.6">
       <c r="A142" s="8" t="s">
         <v>1154</v>
       </c>
@@ -42299,7 +42299,7 @@
       </c>
       <c r="AE142" s="15"/>
     </row>
-    <row r="143" spans="1:31" ht="409.5">
+    <row r="143" spans="1:31" ht="409.6">
       <c r="A143" s="8" t="s">
         <v>161</v>
       </c>
@@ -42366,7 +42366,7 @@
       </c>
       <c r="AE143" s="15"/>
     </row>
-    <row r="144" spans="1:31" ht="409.5">
+    <row r="144" spans="1:31" ht="409.6">
       <c r="A144" s="8" t="s">
         <v>1982</v>
       </c>
@@ -42433,7 +42433,7 @@
       </c>
       <c r="AE144" s="15"/>
     </row>
-    <row r="145" spans="1:31" ht="409.5">
+    <row r="145" spans="1:31" ht="409.6">
       <c r="A145" s="8" t="s">
         <v>722</v>
       </c>
@@ -42500,7 +42500,7 @@
       </c>
       <c r="AE145" s="15"/>
     </row>
-    <row r="146" spans="1:31" ht="409.5">
+    <row r="146" spans="1:31" ht="409.6">
       <c r="A146" s="8" t="s">
         <v>1712</v>
       </c>
@@ -42567,7 +42567,7 @@
       </c>
       <c r="AE146" s="15"/>
     </row>
-    <row r="147" spans="1:31" ht="409.5">
+    <row r="147" spans="1:31" ht="409.6">
       <c r="A147" s="8" t="s">
         <v>938</v>
       </c>
@@ -42634,7 +42634,7 @@
       </c>
       <c r="AE147" s="15"/>
     </row>
-    <row r="148" spans="1:31" ht="409.5">
+    <row r="148" spans="1:31" ht="409.6">
       <c r="A148" s="8" t="s">
         <v>55</v>
       </c>
@@ -42701,7 +42701,7 @@
       </c>
       <c r="AE148" s="15"/>
     </row>
-    <row r="149" spans="1:31" ht="409.5">
+    <row r="149" spans="1:31" ht="409.6">
       <c r="A149" s="8" t="s">
         <v>1757</v>
       </c>
@@ -42768,7 +42768,7 @@
       </c>
       <c r="AE149" s="15"/>
     </row>
-    <row r="150" spans="1:31" ht="409.5">
+    <row r="150" spans="1:31" ht="409.6">
       <c r="A150" s="8" t="s">
         <v>989</v>
       </c>
@@ -42835,7 +42835,7 @@
       </c>
       <c r="AE150" s="15"/>
     </row>
-    <row r="151" spans="1:31" ht="409.5">
+    <row r="151" spans="1:31" ht="409.6">
       <c r="A151" s="8" t="s">
         <v>1934</v>
       </c>
@@ -42902,7 +42902,7 @@
       </c>
       <c r="AE151" s="15"/>
     </row>
-    <row r="152" spans="1:31" ht="409.5">
+    <row r="152" spans="1:31" ht="409.6">
       <c r="A152" s="9" t="s">
         <v>654</v>
       </c>
@@ -42975,7 +42975,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="153" spans="1:31" ht="409.5">
+    <row r="153" spans="1:31" ht="409.6">
       <c r="A153" s="8" t="s">
         <v>190</v>
       </c>
@@ -43042,7 +43042,7 @@
       </c>
       <c r="AE153" s="15"/>
     </row>
-    <row r="154" spans="1:31" ht="409.5">
+    <row r="154" spans="1:31" ht="409.6">
       <c r="A154" s="9" t="s">
         <v>1781</v>
       </c>
@@ -43115,7 +43115,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="155" spans="1:31" ht="409.5">
+    <row r="155" spans="1:31" ht="409.6">
       <c r="A155" s="8" t="s">
         <v>1105</v>
       </c>
@@ -43182,7 +43182,7 @@
       </c>
       <c r="AE155" s="15"/>
     </row>
-    <row r="156" spans="1:31" ht="409.5">
+    <row r="156" spans="1:31" ht="409.6">
       <c r="A156" s="8" t="s">
         <v>2070</v>
       </c>
@@ -43249,7 +43249,7 @@
       </c>
       <c r="AE156" s="15"/>
     </row>
-    <row r="157" spans="1:31" ht="409.5">
+    <row r="157" spans="1:31" ht="409.6">
       <c r="A157" s="8" t="s">
         <v>874</v>
       </c>
@@ -43316,7 +43316,7 @@
       </c>
       <c r="AE157" s="15"/>
     </row>
-    <row r="158" spans="1:31" ht="409.5">
+    <row r="158" spans="1:31" ht="409.6">
       <c r="A158" s="8" t="s">
         <v>297</v>
       </c>
@@ -43383,7 +43383,7 @@
       </c>
       <c r="AE158" s="15"/>
     </row>
-    <row r="159" spans="1:31" ht="409.5">
+    <row r="159" spans="1:31" ht="409.6">
       <c r="A159" s="8" t="s">
         <v>1331</v>
       </c>
@@ -43450,7 +43450,7 @@
       </c>
       <c r="AE159" s="15"/>
     </row>
-    <row r="160" spans="1:31" ht="409.5">
+    <row r="160" spans="1:31" ht="409.6">
       <c r="A160" s="9" t="s">
         <v>2506</v>
       </c>
@@ -43521,7 +43521,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="161" spans="1:32" ht="409.5">
+    <row r="161" spans="1:32" ht="409.6">
       <c r="A161" s="9" t="s">
         <v>1603</v>
       </c>
@@ -43592,7 +43592,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="162" spans="1:32" ht="409.5">
+    <row r="162" spans="1:32" ht="409.6">
       <c r="A162" s="8" t="s">
         <v>2328</v>
       </c>
@@ -43659,7 +43659,7 @@
       </c>
       <c r="AE162" s="15"/>
     </row>
-    <row r="163" spans="1:32" ht="409.5">
+    <row r="163" spans="1:32" ht="409.6">
       <c r="A163" s="8" t="s">
         <v>3072</v>
       </c>
@@ -43726,7 +43726,7 @@
       </c>
       <c r="AE163" s="15"/>
     </row>
-    <row r="164" spans="1:32" ht="409.5">
+    <row r="164" spans="1:32" ht="409.6">
       <c r="A164" s="8" t="s">
         <v>1263</v>
       </c>
@@ -43793,7 +43793,7 @@
       </c>
       <c r="AE164" s="15"/>
     </row>
-    <row r="165" spans="1:32" ht="409.5">
+    <row r="165" spans="1:32" ht="409.6">
       <c r="A165" s="8" t="s">
         <v>2446</v>
       </c>
@@ -43860,7 +43860,7 @@
       </c>
       <c r="AE165" s="15"/>
     </row>
-    <row r="166" spans="1:32" ht="409.5">
+    <row r="166" spans="1:32" ht="409.6">
       <c r="A166" s="9" t="s">
         <v>1474</v>
       </c>
@@ -43934,7 +43934,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="167" spans="1:32" ht="409.5">
+    <row r="167" spans="1:32" ht="409.6">
       <c r="A167" s="8" t="s">
         <v>2141</v>
       </c>
@@ -44001,7 +44001,7 @@
       </c>
       <c r="AE167" s="15"/>
     </row>
-    <row r="168" spans="1:32" ht="409.5">
+    <row r="168" spans="1:32" ht="409.6">
       <c r="A168" s="8" t="s">
         <v>2954</v>
       </c>
@@ -44068,7 +44068,7 @@
       </c>
       <c r="AE168" s="15"/>
     </row>
-    <row r="169" spans="1:32" ht="409.5">
+    <row r="169" spans="1:32" ht="409.6">
       <c r="A169" s="9" t="s">
         <v>1012</v>
       </c>
@@ -44142,7 +44142,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="170" spans="1:32" ht="409.5">
+    <row r="170" spans="1:32" ht="409.6">
       <c r="A170" s="9" t="s">
         <v>1734</v>
       </c>
@@ -44215,7 +44215,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="171" spans="1:32" ht="409.5">
+    <row r="171" spans="1:32" ht="409.6">
       <c r="A171" s="24" t="s">
         <v>676</v>
       </c>
@@ -44289,7 +44289,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="172" spans="1:32" ht="409.5">
+    <row r="172" spans="1:32" ht="409.6">
       <c r="A172" s="9" t="s">
         <v>1903</v>
       </c>
@@ -44363,7 +44363,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="173" spans="1:32" ht="409.5">
+    <row r="173" spans="1:32" ht="409.6">
       <c r="A173" s="9" t="s">
         <v>2593</v>
       </c>
@@ -44439,7 +44439,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="174" spans="1:32" ht="409.5">
+    <row r="174" spans="1:32" ht="409.6">
       <c r="A174" s="8" t="s">
         <v>1081</v>
       </c>
@@ -44506,7 +44506,7 @@
       </c>
       <c r="AE174" s="15"/>
     </row>
-    <row r="175" spans="1:32" ht="409.5">
+    <row r="175" spans="1:32" ht="409.6">
       <c r="A175" s="9" t="s">
         <v>1802</v>
       </c>
@@ -44578,7 +44578,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="176" spans="1:32" ht="409.5">
+    <row r="176" spans="1:32" ht="409.6">
       <c r="A176" s="9" t="s">
         <v>825</v>
       </c>
@@ -44645,7 +44645,7 @@
       </c>
       <c r="AE176" s="15"/>
     </row>
-    <row r="177" spans="1:32" ht="409.5">
+    <row r="177" spans="1:32" ht="409.6">
       <c r="A177" s="8" t="s">
         <v>2104</v>
       </c>
@@ -44714,7 +44714,7 @@
       </c>
       <c r="AE177" s="15"/>
     </row>
-    <row r="178" spans="1:32" ht="409.5">
+    <row r="178" spans="1:32" ht="409.6">
       <c r="A178" s="8" t="s">
         <v>757</v>
       </c>
@@ -44781,7 +44781,7 @@
       </c>
       <c r="AE178" s="15"/>
     </row>
-    <row r="179" spans="1:32" ht="409.5">
+    <row r="179" spans="1:32" ht="409.6">
       <c r="A179" s="8" t="s">
         <v>2039</v>
       </c>
@@ -44848,7 +44848,7 @@
       </c>
       <c r="AE179" s="15"/>
     </row>
-    <row r="180" spans="1:32" ht="409.5">
+    <row r="180" spans="1:32" ht="409.6">
       <c r="A180" s="8" t="s">
         <v>1118</v>
       </c>
@@ -44915,7 +44915,7 @@
       </c>
       <c r="AE180" s="15"/>
     </row>
-    <row r="181" spans="1:32" ht="409.5">
+    <row r="181" spans="1:32" ht="409.6">
       <c r="A181" s="8" t="s">
         <v>1870</v>
       </c>
@@ -44982,7 +44982,7 @@
       </c>
       <c r="AE181" s="15"/>
     </row>
-    <row r="182" spans="1:32" ht="409.5">
+    <row r="182" spans="1:32" ht="409.6">
       <c r="A182" s="8" t="s">
         <v>2781</v>
       </c>
@@ -45051,7 +45051,7 @@
       </c>
       <c r="AE182" s="15"/>
     </row>
-    <row r="183" spans="1:32" ht="409.5">
+    <row r="183" spans="1:32" ht="409.6">
       <c r="A183" s="8" t="s">
         <v>746</v>
       </c>
@@ -45118,7 +45118,7 @@
       </c>
       <c r="AE183" s="15"/>
     </row>
-    <row r="184" spans="1:32" ht="409.5">
+    <row r="184" spans="1:32" ht="409.6">
       <c r="A184" s="8" t="s">
         <v>1956</v>
       </c>
@@ -45187,7 +45187,7 @@
       </c>
       <c r="AE184" s="15"/>
     </row>
-    <row r="185" spans="1:32" ht="409.5">
+    <row r="185" spans="1:32" ht="409.6">
       <c r="A185" s="8" t="s">
         <v>975</v>
       </c>
@@ -45256,7 +45256,7 @@
       </c>
       <c r="AE185" s="15"/>
     </row>
-    <row r="186" spans="1:32" ht="409.5">
+    <row r="186" spans="1:32" ht="409.6">
       <c r="A186" s="8" t="s">
         <v>1685</v>
       </c>
@@ -45325,7 +45325,7 @@
       </c>
       <c r="AE186" s="15"/>
     </row>
-    <row r="187" spans="1:32" ht="409.5">
+    <row r="187" spans="1:32" ht="409.6">
       <c r="A187" s="9" t="s">
         <v>2711</v>
       </c>
@@ -45396,7 +45396,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="188" spans="1:32" ht="409.5">
+    <row r="188" spans="1:32" ht="409.6">
       <c r="A188" s="9" t="s">
         <v>1311</v>
       </c>
@@ -45466,7 +45466,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="189" spans="1:32" ht="409.5">
+    <row r="189" spans="1:32" ht="409.6">
       <c r="A189" s="8" t="s">
         <v>2517</v>
       </c>
@@ -45535,7 +45535,7 @@
       </c>
       <c r="AE189" s="15"/>
     </row>
-    <row r="190" spans="1:32" ht="409.5">
+    <row r="190" spans="1:32" ht="409.6">
       <c r="A190" s="8" t="s">
         <v>1628</v>
       </c>
@@ -45602,7 +45602,7 @@
       </c>
       <c r="AE190" s="15"/>
     </row>
-    <row r="191" spans="1:32" ht="409.5">
+    <row r="191" spans="1:32" ht="409.6">
       <c r="A191" s="9" t="s">
         <v>2316</v>
       </c>
@@ -45671,7 +45671,7 @@
       </c>
       <c r="AE191" s="15"/>
     </row>
-    <row r="192" spans="1:32" ht="409.5">
+    <row r="192" spans="1:32" ht="409.6">
       <c r="A192" s="9" t="s">
         <v>3092</v>
       </c>
@@ -45740,7 +45740,7 @@
       </c>
       <c r="AE192" s="15"/>
     </row>
-    <row r="193" spans="1:31" ht="409.5">
+    <row r="193" spans="1:31" ht="409.6">
       <c r="A193" s="8" t="s">
         <v>1276</v>
       </c>
@@ -45807,7 +45807,7 @@
       </c>
       <c r="AE193" s="15"/>
     </row>
-    <row r="194" spans="1:31" ht="409.5">
+    <row r="194" spans="1:31" ht="409.6">
       <c r="A194" s="8" t="s">
         <v>2426</v>
       </c>
@@ -45876,7 +45876,7 @@
       </c>
       <c r="AE194" s="15"/>
     </row>
-    <row r="195" spans="1:31" ht="409.5">
+    <row r="195" spans="1:31" ht="409.6">
       <c r="A195" s="8" t="s">
         <v>1454</v>
       </c>
@@ -45945,7 +45945,7 @@
       </c>
       <c r="AE195" s="15"/>
     </row>
-    <row r="196" spans="1:31" ht="409.5">
+    <row r="196" spans="1:31" ht="409.6">
       <c r="A196" s="8" t="s">
         <v>2155</v>
       </c>
@@ -46012,7 +46012,7 @@
       </c>
       <c r="AE196" s="15"/>
     </row>
-    <row r="197" spans="1:31" ht="409.5">
+    <row r="197" spans="1:31" ht="409.6">
       <c r="A197" s="8" t="s">
         <v>1533</v>
       </c>
@@ -46081,7 +46081,7 @@
       </c>
       <c r="AE197" s="15"/>
     </row>
-    <row r="198" spans="1:31" ht="409.5">
+    <row r="198" spans="1:31" ht="409.6">
       <c r="A198" s="8" t="s">
         <v>2187</v>
       </c>
@@ -46150,7 +46150,7 @@
       </c>
       <c r="AE198" s="15"/>
     </row>
-    <row r="199" spans="1:31" ht="409.5">
+    <row r="199" spans="1:31" ht="409.6">
       <c r="A199" s="8" t="s">
         <v>1229</v>
       </c>
@@ -46217,7 +46217,7 @@
       </c>
       <c r="AE199" s="15"/>
     </row>
-    <row r="200" spans="1:31" ht="409.5">
+    <row r="200" spans="1:31" ht="409.6">
       <c r="A200" s="8" t="s">
         <v>2381</v>
       </c>
@@ -46284,7 +46284,7 @@
       </c>
       <c r="AE200" s="15"/>
     </row>
-    <row r="201" spans="1:31" ht="409.5">
+    <row r="201" spans="1:31" ht="409.6">
       <c r="A201" s="8" t="s">
         <v>2814</v>
       </c>
@@ -46351,7 +46351,7 @@
       </c>
       <c r="AE201" s="15"/>
     </row>
-    <row r="202" spans="1:31" ht="409.5">
+    <row r="202" spans="1:31" ht="409.6">
       <c r="A202" s="8" t="s">
         <v>2260</v>
       </c>
@@ -46418,7 +46418,7 @@
       </c>
       <c r="AE202" s="15"/>
     </row>
-    <row r="203" spans="1:31" ht="409.5">
+    <row r="203" spans="1:31" ht="409.6">
       <c r="A203" s="8" t="s">
         <v>1353</v>
       </c>
@@ -46485,7 +46485,7 @@
       </c>
       <c r="AE203" s="15"/>
     </row>
-    <row r="204" spans="1:31" ht="409.5">
+    <row r="204" spans="1:31" ht="409.6">
       <c r="A204" s="8" t="s">
         <v>2562</v>
       </c>
@@ -46552,7 +46552,7 @@
       </c>
       <c r="AE204" s="15"/>
     </row>
-    <row r="205" spans="1:31" ht="409.5">
+    <row r="205" spans="1:31" ht="409.6">
       <c r="A205" s="8" t="s">
         <v>2923</v>
       </c>
@@ -46619,7 +46619,7 @@
       </c>
       <c r="AE205" s="15"/>
     </row>
-    <row r="206" spans="1:31" ht="409.5">
+    <row r="206" spans="1:31" ht="409.6">
       <c r="A206" s="8" t="s">
         <v>2004</v>
       </c>
@@ -46686,7 +46686,7 @@
       </c>
       <c r="AE206" s="15"/>
     </row>
-    <row r="207" spans="1:31" ht="409.5">
+    <row r="207" spans="1:31" ht="409.6">
       <c r="A207" s="8" t="s">
         <v>804</v>
       </c>
@@ -46753,7 +46753,7 @@
       </c>
       <c r="AE207" s="15"/>
     </row>
-    <row r="208" spans="1:31" ht="409.5">
+    <row r="208" spans="1:31" ht="409.6">
       <c r="A208" s="8" t="s">
         <v>1856</v>
       </c>
@@ -46820,7 +46820,7 @@
       </c>
       <c r="AE208" s="15"/>
     </row>
-    <row r="209" spans="1:31" ht="409.5">
+    <row r="209" spans="1:31" ht="409.6">
       <c r="A209" s="8" t="s">
         <v>1141</v>
       </c>
@@ -46887,7 +46887,7 @@
       </c>
       <c r="AE209" s="15"/>
     </row>
-    <row r="210" spans="1:31" ht="409.5">
+    <row r="210" spans="1:31" ht="409.6">
       <c r="A210" s="8" t="s">
         <v>1993</v>
       </c>
@@ -46954,7 +46954,7 @@
       </c>
       <c r="AE210" s="15"/>
     </row>
-    <row r="211" spans="1:31" ht="409.5">
+    <row r="211" spans="1:31" ht="409.6">
       <c r="A211" s="8" t="s">
         <v>699</v>
       </c>
@@ -47021,7 +47021,7 @@
       </c>
       <c r="AE211" s="15"/>
     </row>
-    <row r="212" spans="1:31" ht="409.5">
+    <row r="212" spans="1:31" ht="409.6">
       <c r="A212" s="8" t="s">
         <v>1694</v>
       </c>
@@ -47088,7 +47088,7 @@
       </c>
       <c r="AE212" s="15"/>
     </row>
-    <row r="213" spans="1:31" ht="409.5">
+    <row r="213" spans="1:31" ht="409.6">
       <c r="A213" s="8" t="s">
         <v>949</v>
       </c>
@@ -47155,7 +47155,7 @@
       </c>
       <c r="AE213" s="15"/>
     </row>
-    <row r="214" spans="1:31" ht="409.5">
+    <row r="214" spans="1:31" ht="409.6">
       <c r="A214" s="8" t="s">
         <v>26</v>
       </c>
@@ -47222,7 +47222,7 @@
       </c>
       <c r="AE214" s="15"/>
     </row>
-    <row r="215" spans="1:31" ht="409.5">
+    <row r="215" spans="1:31" ht="409.6">
       <c r="A215" s="8" t="s">
         <v>1299</v>
       </c>
@@ -47291,7 +47291,7 @@
       </c>
       <c r="AE215" s="15"/>
     </row>
-    <row r="216" spans="1:31" ht="409.5">
+    <row r="216" spans="1:31" ht="409.6">
       <c r="A216" s="8" t="s">
         <v>1616</v>
       </c>
@@ -47358,7 +47358,7 @@
       </c>
       <c r="AE216" s="15"/>
     </row>
-    <row r="217" spans="1:31" ht="409.5">
+    <row r="217" spans="1:31" ht="409.6">
       <c r="A217" s="9" t="s">
         <v>2304</v>
       </c>
@@ -47431,7 +47431,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="218" spans="1:31" ht="409.5">
+    <row r="218" spans="1:31" ht="409.6">
       <c r="A218" s="8" t="s">
         <v>3083</v>
       </c>
@@ -47498,7 +47498,7 @@
       </c>
       <c r="AE218" s="15"/>
     </row>
-    <row r="219" spans="1:31" ht="409.5">
+    <row r="219" spans="1:31" ht="409.6">
       <c r="A219" s="8" t="s">
         <v>1287</v>
       </c>
@@ -47565,7 +47565,7 @@
       </c>
       <c r="AE219" s="15"/>
     </row>
-    <row r="220" spans="1:31" ht="409.5">
+    <row r="220" spans="1:31" ht="409.6">
       <c r="A220" s="9" t="s">
         <v>2437</v>
       </c>
@@ -47638,7 +47638,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="221" spans="1:31" ht="409.5">
+    <row r="221" spans="1:31" ht="409.6">
       <c r="A221" s="8" t="s">
         <v>1465</v>
       </c>
@@ -47705,7 +47705,7 @@
       </c>
       <c r="AE221" s="15"/>
     </row>
-    <row r="222" spans="1:31" ht="409.5">
+    <row r="222" spans="1:31" ht="409.6">
       <c r="A222" s="8" t="s">
         <v>2167</v>
       </c>
@@ -47772,7 +47772,7 @@
       </c>
       <c r="AE222" s="15"/>
     </row>
-    <row r="223" spans="1:31" ht="409.5">
+    <row r="223" spans="1:31" ht="409.6">
       <c r="A223" s="9" t="s">
         <v>2945</v>
       </c>
@@ -47845,7 +47845,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="224" spans="1:31" ht="409.5">
+    <row r="224" spans="1:31" ht="409.6">
       <c r="A224" s="8" t="s">
         <v>1522</v>
       </c>
@@ -47912,7 +47912,7 @@
       </c>
       <c r="AE224" s="15"/>
     </row>
-    <row r="225" spans="1:31" ht="409.5">
+    <row r="225" spans="1:31" ht="409.6">
       <c r="A225" s="8" t="s">
         <v>2370</v>
       </c>
@@ -47979,7 +47979,7 @@
       </c>
       <c r="AE225" s="15"/>
     </row>
-    <row r="226" spans="1:31" ht="409.5">
+    <row r="226" spans="1:31" ht="409.6">
       <c r="A226" s="8" t="s">
         <v>2803</v>
       </c>
@@ -48046,7 +48046,7 @@
       </c>
       <c r="AE226" s="15"/>
     </row>
-    <row r="227" spans="1:31" ht="409.5">
+    <row r="227" spans="1:31" ht="409.6">
       <c r="A227" s="8" t="s">
         <v>1544</v>
       </c>
@@ -48113,7 +48113,7 @@
       </c>
       <c r="AE227" s="15"/>
     </row>
-    <row r="228" spans="1:31" ht="409.5">
+    <row r="228" spans="1:31" ht="409.6">
       <c r="A228" s="8" t="s">
         <v>2271</v>
       </c>
@@ -48180,7 +48180,7 @@
       </c>
       <c r="AE228" s="15"/>
     </row>
-    <row r="229" spans="1:31" ht="409.5">
+    <row r="229" spans="1:31" ht="409.6">
       <c r="A229" s="8" t="s">
         <v>1364</v>
       </c>
@@ -48247,7 +48247,7 @@
       </c>
       <c r="AE229" s="15"/>
     </row>
-    <row r="230" spans="1:31" ht="409.5">
+    <row r="230" spans="1:31" ht="409.6">
       <c r="A230" s="8" t="s">
         <v>2573</v>
       </c>
@@ -48314,7 +48314,7 @@
       </c>
       <c r="AE230" s="15"/>
     </row>
-    <row r="231" spans="1:31" ht="409.5">
+    <row r="231" spans="1:31" ht="409.6">
       <c r="A231" s="8" t="s">
         <v>2934</v>
       </c>
@@ -48381,7 +48381,7 @@
       </c>
       <c r="AE231" s="15"/>
     </row>
-    <row r="232" spans="1:31" ht="409.5">
+    <row r="232" spans="1:31" ht="409.6">
       <c r="A232" s="8" t="s">
         <v>1025</v>
       </c>
@@ -48448,7 +48448,7 @@
       </c>
       <c r="AE232" s="15"/>
     </row>
-    <row r="233" spans="1:31" ht="409.5">
+    <row r="233" spans="1:31" ht="409.6">
       <c r="A233" s="8" t="s">
         <v>1745</v>
       </c>
@@ -48515,7 +48515,7 @@
       </c>
       <c r="AE233" s="15"/>
     </row>
-    <row r="234" spans="1:31" ht="409.5">
+    <row r="234" spans="1:31" ht="409.6">
       <c r="A234" s="8" t="s">
         <v>688</v>
       </c>
@@ -48582,7 +48582,7 @@
       </c>
       <c r="AE234" s="15"/>
     </row>
-    <row r="235" spans="1:31" ht="409.5">
+    <row r="235" spans="1:31" ht="409.6">
       <c r="A235" s="8" t="s">
         <v>1912</v>
       </c>
@@ -48649,7 +48649,7 @@
       </c>
       <c r="AE235" s="15"/>
     </row>
-    <row r="236" spans="1:31" ht="409.5">
+    <row r="236" spans="1:31" ht="409.6">
       <c r="A236" s="8" t="s">
         <v>2604</v>
       </c>
@@ -48716,7 +48716,7 @@
       </c>
       <c r="AE236" s="15"/>
     </row>
-    <row r="237" spans="1:31" ht="409.5">
+    <row r="237" spans="1:31" ht="409.6">
       <c r="A237" s="8" t="s">
         <v>1070</v>
       </c>
@@ -48783,7 +48783,7 @@
       </c>
       <c r="AE237" s="15"/>
     </row>
-    <row r="238" spans="1:31" ht="409.5">
+    <row r="238" spans="1:31" ht="409.6">
       <c r="A238" s="8" t="s">
         <v>1792</v>
       </c>
@@ -48850,7 +48850,7 @@
       </c>
       <c r="AE238" s="15"/>
     </row>
-    <row r="239" spans="1:31" ht="409.5">
+    <row r="239" spans="1:31" ht="409.6">
       <c r="A239" s="8" t="s">
         <v>815</v>
       </c>
@@ -48917,7 +48917,7 @@
       </c>
       <c r="AE239" s="15"/>
     </row>
-    <row r="240" spans="1:31" ht="409.5">
+    <row r="240" spans="1:31" ht="409.6">
       <c r="A240" s="8" t="s">
         <v>2092</v>
       </c>
@@ -48984,7 +48984,7 @@
       </c>
       <c r="AE240" s="15"/>
     </row>
-    <row r="241" spans="1:31" ht="409.5">
+    <row r="241" spans="1:31" ht="409.6">
       <c r="A241" s="8" t="s">
         <v>2680</v>
       </c>
@@ -49051,7 +49051,7 @@
       </c>
       <c r="AE241" s="15"/>
     </row>
-    <row r="242" spans="1:31" ht="409.5">
+    <row r="242" spans="1:31" ht="409.6">
       <c r="A242" s="8" t="s">
         <v>768</v>
       </c>
@@ -49118,7 +49118,7 @@
       </c>
       <c r="AE242" s="15"/>
     </row>
-    <row r="243" spans="1:31" ht="409.5">
+    <row r="243" spans="1:31" ht="409.6">
       <c r="A243" s="8" t="s">
         <v>2050</v>
       </c>
@@ -49185,7 +49185,7 @@
       </c>
       <c r="AE243" s="15"/>
     </row>
-    <row r="244" spans="1:31" ht="409.5">
+    <row r="244" spans="1:31" ht="409.6">
       <c r="A244" s="8" t="s">
         <v>1129</v>
       </c>
@@ -49252,7 +49252,7 @@
       </c>
       <c r="AE244" s="15"/>
     </row>
-    <row r="245" spans="1:31" ht="409.5">
+    <row r="245" spans="1:31" ht="409.6">
       <c r="A245" s="8" t="s">
         <v>1883</v>
       </c>
@@ -49319,7 +49319,7 @@
       </c>
       <c r="AE245" s="15"/>
     </row>
-    <row r="246" spans="1:31" ht="409.5">
+    <row r="246" spans="1:31" ht="409.6">
       <c r="A246" s="8" t="s">
         <v>2792</v>
       </c>
@@ -49386,7 +49386,7 @@
       </c>
       <c r="AE246" s="15"/>
     </row>
-    <row r="247" spans="1:31" ht="409.5">
+    <row r="247" spans="1:31" ht="409.6">
       <c r="A247" s="8" t="s">
         <v>735</v>
       </c>
@@ -49453,7 +49453,7 @@
       </c>
       <c r="AE247" s="15"/>
     </row>
-    <row r="248" spans="1:31" ht="409.5">
+    <row r="248" spans="1:31" ht="409.6">
       <c r="A248" s="8" t="s">
         <v>1945</v>
       </c>
@@ -49520,7 +49520,7 @@
       </c>
       <c r="AE248" s="15"/>
     </row>
-    <row r="249" spans="1:31" ht="409.5">
+    <row r="249" spans="1:31" ht="409.6">
       <c r="A249" s="8" t="s">
         <v>961</v>
       </c>
@@ -49587,7 +49587,7 @@
       </c>
       <c r="AE249" s="15"/>
     </row>
-    <row r="250" spans="1:31" ht="409.5">
+    <row r="250" spans="1:31" ht="409.6">
       <c r="A250" s="8" t="s">
         <v>1674</v>
       </c>
@@ -49654,7 +49654,7 @@
       </c>
       <c r="AE250" s="15"/>
     </row>
-    <row r="251" spans="1:31" ht="409.5">
+    <row r="251" spans="1:31" ht="409.6">
       <c r="A251" s="8" t="s">
         <v>2700</v>
       </c>
@@ -49721,7 +49721,7 @@
       </c>
       <c r="AE251" s="15"/>
     </row>
-    <row r="252" spans="1:31" ht="409.5">
+    <row r="252" spans="1:31" ht="409.6">
       <c r="A252" s="8" t="s">
         <v>2198</v>
       </c>
@@ -49788,7 +49788,7 @@
       </c>
       <c r="AE252" s="15"/>
     </row>
-    <row r="253" spans="1:31" ht="409.5">
+    <row r="253" spans="1:31" ht="409.6">
       <c r="A253" s="8" t="s">
         <v>1511</v>
       </c>
@@ -49855,7 +49855,7 @@
       </c>
       <c r="AE253" s="15"/>
     </row>
-    <row r="254" spans="1:31" ht="409.5">
+    <row r="254" spans="1:31" ht="409.6">
       <c r="A254" s="8" t="s">
         <v>2415</v>
       </c>
@@ -49922,7 +49922,7 @@
       </c>
       <c r="AE254" s="15"/>
     </row>
-    <row r="255" spans="1:31" ht="409.5">
+    <row r="255" spans="1:31" ht="409.6">
       <c r="A255" s="8" t="s">
         <v>1196</v>
       </c>
@@ -49989,7 +49989,7 @@
       </c>
       <c r="AE255" s="15"/>
     </row>
-    <row r="256" spans="1:31" ht="409.5">
+    <row r="256" spans="1:31" ht="409.6">
       <c r="A256" s="8" t="s">
         <v>488</v>
       </c>
@@ -50056,7 +50056,7 @@
       </c>
       <c r="AE256" s="15"/>
     </row>
-    <row r="257" spans="1:31" ht="409.5">
+    <row r="257" spans="1:31" ht="409.6">
       <c r="A257" s="8" t="s">
         <v>2249</v>
       </c>
@@ -50123,7 +50123,7 @@
       </c>
       <c r="AE257" s="15"/>
     </row>
-    <row r="258" spans="1:31" ht="409.5">
+    <row r="258" spans="1:31" ht="409.6">
       <c r="A258" s="8" t="s">
         <v>1555</v>
       </c>
@@ -50192,7 +50192,7 @@
       </c>
       <c r="AE258" s="15"/>
     </row>
-    <row r="259" spans="1:31" ht="409.5">
+    <row r="259" spans="1:31" ht="409.6">
       <c r="A259" s="8" t="s">
         <v>2528</v>
       </c>
@@ -50259,7 +50259,7 @@
       </c>
       <c r="AE259" s="15"/>
     </row>
-    <row r="260" spans="1:31" ht="409.5">
+    <row r="260" spans="1:31" ht="409.6">
       <c r="A260" s="8" t="s">
         <v>1384</v>
       </c>
@@ -50326,7 +50326,7 @@
       </c>
       <c r="AE260" s="15"/>
     </row>
-    <row r="261" spans="1:31" ht="409.5">
+    <row r="261" spans="1:31" ht="409.6">
       <c r="A261" s="8" t="s">
         <v>609</v>
       </c>
@@ -50393,7 +50393,7 @@
       </c>
       <c r="AE261" s="15"/>
     </row>
-    <row r="262" spans="1:31" ht="409.5">
+    <row r="262" spans="1:31" ht="409.6">
       <c r="A262" s="8" t="s">
         <v>1811</v>
       </c>
@@ -50460,7 +50460,7 @@
       </c>
       <c r="AE262" s="15"/>
     </row>
-    <row r="263" spans="1:31" ht="409.5">
+    <row r="263" spans="1:31" ht="409.6">
       <c r="A263" s="8" t="s">
         <v>1059</v>
       </c>
@@ -50527,7 +50527,7 @@
       </c>
       <c r="AE263" s="15"/>
     </row>
-    <row r="264" spans="1:31" ht="409.5">
+    <row r="264" spans="1:31" ht="409.6">
       <c r="A264" s="8" t="s">
         <v>838</v>
       </c>
@@ -50594,7 +50594,7 @@
       </c>
       <c r="AE264" s="15"/>
     </row>
-    <row r="265" spans="1:31" ht="409.5">
+    <row r="265" spans="1:31" ht="409.6">
       <c r="A265" s="8" t="s">
         <v>309</v>
       </c>
@@ -50661,7 +50661,7 @@
       </c>
       <c r="AE265" s="15"/>
     </row>
-    <row r="266" spans="1:31" ht="409.5">
+    <row r="266" spans="1:31" ht="409.6">
       <c r="A266" s="8" t="s">
         <v>1591</v>
       </c>
@@ -50728,7 +50728,7 @@
       </c>
       <c r="AE266" s="15"/>
     </row>
-    <row r="267" spans="1:31" ht="409.5">
+    <row r="267" spans="1:31" ht="409.6">
       <c r="A267" s="8" t="s">
         <v>2495</v>
       </c>
@@ -50795,7 +50795,7 @@
       </c>
       <c r="AE267" s="15"/>
     </row>
-    <row r="268" spans="1:31" ht="409.5">
+    <row r="268" spans="1:31" ht="409.6">
       <c r="A268" s="8" t="s">
         <v>1320</v>
       </c>
@@ -50862,7 +50862,7 @@
       </c>
       <c r="AE268" s="15"/>
     </row>
-    <row r="269" spans="1:31" ht="409.5">
+    <row r="269" spans="1:31" ht="409.6">
       <c r="A269" s="8" t="s">
         <v>2359</v>
       </c>
@@ -50929,7 +50929,7 @@
       </c>
       <c r="AE269" s="15"/>
     </row>
-    <row r="270" spans="1:31" ht="409.5">
+    <row r="270" spans="1:31" ht="409.6">
       <c r="A270" s="8" t="s">
         <v>1663</v>
       </c>
@@ -50996,7 +50996,7 @@
       </c>
       <c r="AE270" s="15"/>
     </row>
-    <row r="271" spans="1:31" ht="409.5">
+    <row r="271" spans="1:31" ht="409.6">
       <c r="A271" s="8" t="s">
         <v>378</v>
       </c>
@@ -51063,7 +51063,7 @@
       </c>
       <c r="AE271" s="15"/>
     </row>
-    <row r="272" spans="1:31" ht="409.5">
+    <row r="272" spans="1:31" ht="409.6">
       <c r="A272" s="8" t="s">
         <v>2348</v>
       </c>
@@ -51130,7 +51130,7 @@
       </c>
       <c r="AE272" s="15"/>
     </row>
-    <row r="273" spans="1:31" ht="409.5">
+    <row r="273" spans="1:31" ht="409.6">
       <c r="A273" s="8" t="s">
         <v>3104</v>
       </c>

</xml_diff>

<commit_message>
update tracker and overlay for 73595, 73601, 73613
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-high-microsoft-windows-server-2016-stig-overlay.xlsx
+++ b/cms-ars-3.1-high-microsoft-windows-server-2016-stig-overlay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishna/Documents/Projects/CMS/Inspec/STIG_Profiles/microsoft-windows-server-2016/cms-ars-3.1-high-microsoft-windows-server-2016-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BED612-AE70-EF48-8A83-498F8B4019AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DFCC4D-FED8-6F44-A505-E88885ED10F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-high-microsoft-wind" sheetId="1" r:id="rId1"/>
@@ -29015,105 +29015,6 @@
 an organization-defined equivalent.
 If an organization-defined title is used, it can in no case contravene or
 modify the language of the message text required in WN16-SO-000150.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This applies to domain controllers. It is NA for other systems.
-Run "MMC".
-Select "Add/Remove Snap-in" from the "File" menu.
-Select "Certificates" in the left pane and click the "Add &gt;" button.
-Select "Computer Account" and click "Next".
-Select the appropriate option for "Select the computer you want this snap-in
-to manage" and click "Finish".
-Click "OK".
-Select and expand the Certificates (Local Computer) entry in the left pane.
-Select and expand the Personal entry in the left pane.
-Select the Certificates entry in the left pane.
-In the right pane, examine the "Issued By" field for the certificate to
-determine the issuing CA.
-If the "Issued By" field of the PKI certificate being used by the domain
-controller does not indicate the issuing CA is part of the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>DoD</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> CMS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> PKI or an
-approved ECA, this is a finding.
-If the certificates in use are issued by a CA authorized by the Component's
-CIO, this is a CAT II finding.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">There are multiple sources from which lists of valid </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>DoD</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> CMS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> CAs and approved ECAs
-can be obtained:
-The Global Directory Service (GDS) website provides an online source. The
-address for this site is https://crl.gds.disa.mil.
-DoD CMS Public Key Enablement (PKE) Engineering Support maintains the InstallRoot
-utility to manage DoD CMS supported root certificates on Windows computers, which
-includes a list of authorized CAs. The utility package can be downloaded from
-the PKI and PKE Tools page on IASE:
-http://iase.disa.mil/pki-pke/function_pages/tools.html</t>
     </r>
   </si>
   <si>
@@ -31359,12 +31260,106 @@
 which is unacceptable).</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This applies to domain controllers. It is NA for other systems.
+Run "MMC".
+Select "Add/Remove Snap-in" from the "File" menu.
+Select "Certificates" in the left pane and click the "Add &gt;" button.
+Select "Computer Account" and click "Next".
+Select the appropriate option for "Select the computer you want this snap-in
+to manage" and click "Finish".
+Click "OK".
+Select and expand the Certificates (Local Computer) entry in the left pane.
+Select and expand the Personal entry in the left pane.
+Select the Certificates entry in the left pane.
+In the right pane, examine the "Issued By" field for the certificate to
+determine the issuing CA.
+If the "Issued By" field of the PKI certificate being used by the domain
+controller does not indicate the issuing CA is part of the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>DoD</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> CMS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> PKI or an
+approved ECA, this is a finding.
+If the certificates in use are issued by a CA authorized by the Component's
+CIO, this is a CAT II finding.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+There are multiple sources from which lists of valid </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>DoD CMS</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CAs and approved ECAs
+can be obtained:
+The Global Directory Service (GDS) website provides an online source. The
+address for this site is https://crl.gds.disa.mil.
+DoD CMS Public Key Enablement (PKE) Engineering Support maintains the InstallRoot
+utility to manage DoD CMS supported root certificates on Windows computers, which
+includes a list of authorized CAs. The utility package can be downloaded from
+the PKI and PKE Tools page on IASE:
+http://iase.disa.mil/pki-pke/function_pages/tools.html</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="47">
+  <fonts count="48">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -31707,6 +31702,15 @@
     <font>
       <sz val="24"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -32592,8 +32596,8 @@
   <dimension ref="A1:AF273"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E188" sqref="E188"/>
+      <pane ySplit="1" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X176" sqref="X176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="31"/>
@@ -33121,10 +33125,10 @@
         <v>0.5</v>
       </c>
       <c r="D8" s="14" t="s">
+        <v>3150</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>3151</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>3152</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>629</v>
@@ -33159,10 +33163,10 @@
       <c r="V8" s="13"/>
       <c r="W8" s="13"/>
       <c r="X8" s="14" t="s">
+        <v>3152</v>
+      </c>
+      <c r="Y8" s="14" t="s">
         <v>3153</v>
-      </c>
-      <c r="Y8" s="14" t="s">
-        <v>3154</v>
       </c>
       <c r="Z8" s="14" t="s">
         <v>637</v>
@@ -33188,7 +33192,7 @@
         <v>0.5</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>3173</v>
+        <v>3172</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>2761</v>
@@ -33226,10 +33230,10 @@
       <c r="V9" s="13"/>
       <c r="W9" s="13"/>
       <c r="X9" s="25" t="s">
-        <v>3175</v>
+        <v>3174</v>
       </c>
       <c r="Y9" s="25" t="s">
-        <v>3174</v>
+        <v>3173</v>
       </c>
       <c r="Z9" s="14" t="s">
         <v>2767</v>
@@ -33246,7 +33250,7 @@
       </c>
       <c r="AE9" s="15"/>
       <c r="AF9" s="27" t="s">
-        <v>3172</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="409.6">
@@ -34110,10 +34114,10 @@
       <c r="V22" s="13"/>
       <c r="W22" s="13"/>
       <c r="X22" s="16" t="s">
+        <v>3148</v>
+      </c>
+      <c r="Y22" s="16" t="s">
         <v>3149</v>
-      </c>
-      <c r="Y22" s="16" t="s">
-        <v>3150</v>
       </c>
       <c r="Z22" s="14" t="s">
         <v>1401</v>
@@ -34756,10 +34760,10 @@
         <v>0.5</v>
       </c>
       <c r="D32" s="25" t="s">
+        <v>3175</v>
+      </c>
+      <c r="E32" s="25" t="s">
         <v>3176</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>3177</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>108</v>
@@ -34794,10 +34798,10 @@
       <c r="V32" s="13"/>
       <c r="W32" s="13"/>
       <c r="X32" s="28" t="s">
+        <v>3177</v>
+      </c>
+      <c r="Y32" s="28" t="s">
         <v>3178</v>
-      </c>
-      <c r="Y32" s="28" t="s">
-        <v>3179</v>
       </c>
       <c r="Z32" s="14" t="s">
         <v>116</v>
@@ -34814,7 +34818,7 @@
       </c>
       <c r="AE32" s="15"/>
       <c r="AF32" s="27" t="s">
-        <v>3172</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="33" spans="1:32" ht="409.6">
@@ -34826,7 +34830,7 @@
         <v>0.5</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>3162</v>
+        <v>3161</v>
       </c>
       <c r="E33" s="16" t="s">
         <v>3130</v>
@@ -34931,7 +34935,7 @@
       <c r="V34" s="13"/>
       <c r="W34" s="13"/>
       <c r="X34" s="30" t="s">
-        <v>3180</v>
+        <v>3179</v>
       </c>
       <c r="Y34" s="16" t="s">
         <v>3134</v>
@@ -34951,7 +34955,7 @@
       </c>
       <c r="AE34" s="15"/>
       <c r="AF34" s="27" t="s">
-        <v>3172</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="35" spans="1:32" ht="409.6">
@@ -35671,10 +35675,10 @@
       <c r="V45" s="13"/>
       <c r="W45" s="13"/>
       <c r="X45" s="25" t="s">
+        <v>3180</v>
+      </c>
+      <c r="Y45" s="25" t="s">
         <v>3181</v>
-      </c>
-      <c r="Y45" s="25" t="s">
-        <v>3182</v>
       </c>
       <c r="Z45" s="14" t="s">
         <v>505</v>
@@ -35691,7 +35695,7 @@
       </c>
       <c r="AE45" s="15"/>
       <c r="AF45" s="27" t="s">
-        <v>3172</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="46" spans="1:32" ht="409.6">
@@ -35906,10 +35910,10 @@
         <v>0.5</v>
       </c>
       <c r="D49" s="16" t="s">
+        <v>3157</v>
+      </c>
+      <c r="E49" s="16" t="s">
         <v>3158</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>3159</v>
       </c>
       <c r="F49" s="13" t="s">
         <v>2910</v>
@@ -35944,10 +35948,10 @@
       <c r="V49" s="13"/>
       <c r="W49" s="13"/>
       <c r="X49" s="16" t="s">
+        <v>3159</v>
+      </c>
+      <c r="Y49" s="16" t="s">
         <v>3160</v>
-      </c>
-      <c r="Y49" s="16" t="s">
-        <v>3161</v>
       </c>
       <c r="Z49" s="14" t="s">
         <v>2918</v>
@@ -36107,7 +36111,7 @@
         <v>0.5</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>3155</v>
+        <v>3154</v>
       </c>
       <c r="E52" s="14" t="s">
         <v>2866</v>
@@ -36145,10 +36149,10 @@
       <c r="V52" s="13"/>
       <c r="W52" s="13"/>
       <c r="X52" s="16" t="s">
+        <v>3155</v>
+      </c>
+      <c r="Y52" s="16" t="s">
         <v>3156</v>
-      </c>
-      <c r="Y52" s="16" t="s">
-        <v>3157</v>
       </c>
       <c r="Z52" s="14" t="s">
         <v>2872</v>
@@ -37258,7 +37262,7 @@
         <v>0.3</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>3146</v>
+        <v>3145</v>
       </c>
       <c r="E69" s="14" t="s">
         <v>3057</v>
@@ -37296,10 +37300,10 @@
       <c r="V69" s="13"/>
       <c r="W69" s="13"/>
       <c r="X69" s="16" t="s">
+        <v>3146</v>
+      </c>
+      <c r="Y69" s="16" t="s">
         <v>3147</v>
-      </c>
-      <c r="Y69" s="16" t="s">
-        <v>3148</v>
       </c>
       <c r="Z69" s="14" t="s">
         <v>3066</v>
@@ -43925,13 +43929,13 @@
         <v>1016</v>
       </c>
       <c r="AD166" s="28" t="s">
+        <v>3182</v>
+      </c>
+      <c r="AE166" s="28" t="s">
         <v>3183</v>
       </c>
-      <c r="AE166" s="28" t="s">
-        <v>3184</v>
-      </c>
       <c r="AF166" s="27" t="s">
-        <v>3172</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="167" spans="1:32" ht="409.6">
@@ -44133,13 +44137,13 @@
         <v>1016</v>
       </c>
       <c r="AD169" s="28" t="s">
+        <v>3182</v>
+      </c>
+      <c r="AE169" s="28" t="s">
         <v>3183</v>
       </c>
-      <c r="AE169" s="28" t="s">
-        <v>3184</v>
-      </c>
       <c r="AF169" s="27" t="s">
-        <v>3172</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="170" spans="1:32" ht="409.6">
@@ -44224,10 +44228,10 @@
         <v>0.5</v>
       </c>
       <c r="D171" s="19" t="s">
-        <v>3163</v>
+        <v>3162</v>
       </c>
       <c r="E171" s="19" t="s">
-        <v>3165</v>
+        <v>3164</v>
       </c>
       <c r="F171" s="14" t="s">
         <v>674</v>
@@ -44262,10 +44266,10 @@
       <c r="V171" s="14"/>
       <c r="W171" s="14"/>
       <c r="X171" s="19" t="s">
-        <v>3164</v>
+        <v>3163</v>
       </c>
       <c r="Y171" s="19" t="s">
-        <v>3166</v>
+        <v>3165</v>
       </c>
       <c r="Z171" s="14" t="s">
         <v>682</v>
@@ -44286,7 +44290,7 @@
         <v>3123</v>
       </c>
       <c r="AF171" s="27" t="s">
-        <v>3172</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="172" spans="1:32" ht="409.6">
@@ -44298,10 +44302,10 @@
         <v>0.5</v>
       </c>
       <c r="D172" s="19" t="s">
+        <v>3166</v>
+      </c>
+      <c r="E172" s="19" t="s">
         <v>3167</v>
-      </c>
-      <c r="E172" s="19" t="s">
-        <v>3168</v>
       </c>
       <c r="F172" s="19" t="s">
         <v>1902</v>
@@ -44336,10 +44340,10 @@
       <c r="V172" s="19"/>
       <c r="W172" s="19"/>
       <c r="X172" s="19" t="s">
+        <v>3168</v>
+      </c>
+      <c r="Y172" s="19" t="s">
         <v>3169</v>
-      </c>
-      <c r="Y172" s="19" t="s">
-        <v>3170</v>
       </c>
       <c r="Z172" s="19" t="s">
         <v>1907</v>
@@ -44360,7 +44364,7 @@
         <v>3123</v>
       </c>
       <c r="AF172" s="27" t="s">
-        <v>3172</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="173" spans="1:32" ht="409.6">
@@ -44433,10 +44437,10 @@
         <v>681</v>
       </c>
       <c r="AE173" s="12" t="s">
+        <v>3170</v>
+      </c>
+      <c r="AF173" s="27" t="s">
         <v>3171</v>
-      </c>
-      <c r="AF173" s="27" t="s">
-        <v>3172</v>
       </c>
     </row>
     <row r="174" spans="1:32" ht="409.6">
@@ -44553,7 +44557,7 @@
       <c r="V175" s="13"/>
       <c r="W175" s="13"/>
       <c r="X175" s="23" t="s">
-        <v>3145</v>
+        <v>3188</v>
       </c>
       <c r="Y175" s="16" t="s">
         <v>3127</v>
@@ -44575,7 +44579,7 @@
         <v>3123</v>
       </c>
       <c r="AF175" s="27" t="s">
-        <v>3172</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="176" spans="1:32" ht="409.6">
@@ -45405,10 +45409,10 @@
         <v>0.5</v>
       </c>
       <c r="D188" s="25" t="s">
+        <v>3184</v>
+      </c>
+      <c r="E188" s="30" t="s">
         <v>3185</v>
-      </c>
-      <c r="E188" s="30" t="s">
-        <v>3186</v>
       </c>
       <c r="F188" s="29" t="s">
         <v>1310</v>
@@ -45443,10 +45447,10 @@
       <c r="V188" s="29"/>
       <c r="W188" s="29"/>
       <c r="X188" s="30" t="s">
+        <v>3186</v>
+      </c>
+      <c r="Y188" s="30" t="s">
         <v>3187</v>
-      </c>
-      <c r="Y188" s="30" t="s">
-        <v>3188</v>
       </c>
       <c r="Z188" s="14" t="s">
         <v>1315</v>
@@ -45463,7 +45467,7 @@
       </c>
       <c r="AE188" s="15"/>
       <c r="AF188" s="27" t="s">
-        <v>3172</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="189" spans="1:32" ht="409.6">

</xml_diff>